<commit_message>
Added VC++ Project to Folder, xls update
</commit_message>
<xml_diff>
--- a/DrogoTimeTracking.xlsx
+++ b/DrogoTimeTracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supervisor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supervisor\Desktop\DrogoEngine\DrogoEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t>Monday</t>
   </si>
@@ -122,7 +122,16 @@
     <t>Total Working Hours</t>
   </si>
   <si>
-    <t>Starting up GitHub, Creating Time Tracking File. Getting Surfaces on the Screen and Keyboard Input functions.</t>
+    <t>Starting up GitHub, Creating Time Tracking File. Setting up SDL and SDL_Image, getting Keyboard Input and loading image different image formats as surfaces. Learning about SDL renderer, texturing and viewports.</t>
+  </si>
+  <si>
+    <t>Modulating Color and Alpha with rgba components in the renderer. Animating, Rotating and Flipping with SDL. Re-organizing scripts. On-mouse events.</t>
+  </si>
+  <si>
+    <t>Modulating Color and Alpha with rgba components in the renderer. Animating, Rotating and Flipping with SDL. Displaying truetype fonts in the screen. Re-organizing scripts. On-mouse events.</t>
+  </si>
+  <si>
+    <t>Starting up GitHub, Creating Time Tracking File. Setting up SDL and SDL_Image. Getting Keyboard Input. Loading image different image formats as surfaces. Learning about SDL renderer and texturing. Using viewports.</t>
   </si>
 </sst>
 </file>
@@ -188,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +279,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFBEF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,15 +334,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -357,6 +363,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,6 +383,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFBEF"/>
       <color rgb="FFFFFF00"/>
     </mruColors>
   </colors>
@@ -645,7 +664,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,98 +676,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="F1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="11"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10">
+      <c r="A5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="18">
+        <v>9</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7">
         <f>SUM(B5:H5)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10">
+      <c r="A7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7">
         <f>SUM(B7:H7)</f>
         <v>0</v>
       </c>
@@ -757,27 +780,27 @@
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10">
+      <c r="A9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7">
         <f>SUM(B9:H9)</f>
         <v>0</v>
       </c>
@@ -786,27 +809,27 @@
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10">
+      <c r="A11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7">
         <f>SUM(B11:H11)</f>
         <v>0</v>
       </c>
@@ -815,27 +838,27 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10">
+      <c r="A13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7">
         <f>SUM(B13:H13)</f>
         <v>0</v>
       </c>
@@ -844,27 +867,27 @@
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10">
+      <c r="A15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7">
         <f>SUM(B15:H15)</f>
         <v>0</v>
       </c>
@@ -873,27 +896,27 @@
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10">
+      <c r="A17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7">
         <f>SUM(B17:H17)</f>
         <v>0</v>
       </c>
@@ -902,27 +925,27 @@
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10">
+      <c r="A19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7">
         <f>SUM(B19:H19)</f>
         <v>0</v>
       </c>
@@ -931,27 +954,27 @@
       <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="22"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10">
+      <c r="A21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7">
         <f>SUM(B21:H21)</f>
         <v>0</v>
       </c>
@@ -960,27 +983,27 @@
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10">
+      <c r="A23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7">
         <f>SUM(B23:H23)</f>
         <v>0</v>
       </c>
@@ -989,27 +1012,27 @@
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10">
+      <c r="A25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7">
         <f>SUM(B25:H25)</f>
         <v>0</v>
       </c>
@@ -1018,27 +1041,27 @@
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10">
+      <c r="A27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7">
         <f>SUM(B27:H27)</f>
         <v>0</v>
       </c>
@@ -1047,27 +1070,27 @@
       <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10">
+      <c r="A29" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7">
         <f>SUM(B29:H29)</f>
         <v>0</v>
       </c>
@@ -1076,27 +1099,27 @@
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10">
+      <c r="A31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7">
         <f>SUM(B31:H31)</f>
         <v>0</v>
       </c>
@@ -1105,27 +1128,27 @@
       <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10">
+      <c r="A33" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7">
         <f>SUM(B33:H33)</f>
         <v>0</v>
       </c>
@@ -1134,27 +1157,27 @@
       <c r="A34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10">
+      <c r="A35" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7">
         <f>SUM(B35:H35)</f>
         <v>0</v>
       </c>
@@ -1163,27 +1186,27 @@
       <c r="A36" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="10">
+      <c r="A37" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="7">
         <f>SUM(B37:H37)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Ported Engine to Folder, Updated Timetracking File
</commit_message>
<xml_diff>
--- a/DrogoTimeTracking.xlsx
+++ b/DrogoTimeTracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supervisor\Desktop\DrogoEngine\DrogoEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supervisor\Desktop\DrogoEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Monday</t>
   </si>
@@ -127,6 +126,12 @@
   </si>
   <si>
     <t>Starting up GitHub, Creating Time Tracking File. Setting up SDL and SDL_Image. Getting Keyboard Input. Loading image different image formats as surfaces. Learning about SDL renderer and texturing. Using viewports.</t>
+  </si>
+  <si>
+    <t>On-mouse events, reorganizing code, using SDL_mixer for sound.</t>
+  </si>
+  <si>
+    <t>Making buttons play sounds. Using Timing as a counter and to count frames. Capping fps. Collision detections (Squared, Circular and Per-Pixel).</t>
   </si>
 </sst>
 </file>
@@ -659,7 +664,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,7 +725,9 @@
       <c r="F4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
@@ -734,19 +741,25 @@
       <c r="E5" s="18">
         <v>9</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="F5" s="18">
+        <v>9</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7">
         <f>SUM(B5:H5)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>

</xml_diff>